<commit_message>
travel request view detail continue
</commit_message>
<xml_diff>
--- a/data/JGI-MS-HRIS.xlsx
+++ b/data/JGI-MS-HRIS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
   <si>
     <t xml:space="preserve">SN</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t xml:space="preserve">                   nepali date and english date </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   to do list</t>
   </si>
 </sst>
 </file>
@@ -197,6 +200,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -219,6 +223,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -270,7 +275,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -280,7 +285,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -292,19 +297,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -324,18 +325,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="83.6599190283401"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.59109311740891"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="84.4089068825911"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.63967611336032"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -435,7 +436,7 @@
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="1"/>
@@ -449,7 +450,7 @@
       <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1"/>
@@ -463,7 +464,7 @@
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="1"/>
@@ -477,7 +478,7 @@
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="1"/>
@@ -491,7 +492,7 @@
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="1"/>
@@ -505,7 +506,7 @@
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="1"/>
@@ -519,7 +520,7 @@
       <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="1"/>
@@ -547,7 +548,7 @@
       <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -563,7 +564,7 @@
       <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -579,7 +580,7 @@
       <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -595,7 +596,7 @@
       <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -613,7 +614,7 @@
       <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -629,7 +630,7 @@
       <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -645,7 +646,7 @@
       <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -661,7 +662,7 @@
       <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -677,7 +678,7 @@
       <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C23" s="1"/>
@@ -691,7 +692,7 @@
       <c r="A24" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C24" s="1"/>
@@ -705,7 +706,7 @@
       <c r="A25" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C25" s="1"/>
@@ -719,7 +720,7 @@
       <c r="A26" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>35</v>
       </c>
       <c r="C26" s="1"/>
@@ -835,7 +836,7 @@
       <c r="A33" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C33" s="1"/>
@@ -867,7 +868,7 @@
       <c r="A35" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>44</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -885,7 +886,7 @@
       <c r="A36" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>46</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -901,7 +902,7 @@
       <c r="A37" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="7" t="s">
         <v>47</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -917,7 +918,7 @@
       <c r="A38" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -933,7 +934,7 @@
       <c r="A39" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="7" t="s">
         <v>49</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -953,7 +954,7 @@
       <c r="A40" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="7" t="s">
         <v>51</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -974,6 +975,11 @@
       </c>
       <c r="C41" s="0" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>